<commit_message>
Fixing conflict of intents First (not yet tested) steps to align CreateUniqueIntent with toIntent
</commit_message>
<xml_diff>
--- a/example/cz_app/xls/E_CZ_master.xlsx
+++ b/example/cz_app/xls/E_CZ_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tom\Watson\public_workspaces\watson-assistant-workbench\example\cz_app\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2830745-A840-4417-BA7D-17881117FCF8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10BBEE2-B992-4CB4-926D-926A7C1AA85F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KLABOSENI" sheetId="2" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>// TLAČÍTKA</t>
   </si>
   <si>
-    <t>#CO_JE</t>
-  </si>
-  <si>
     <t xml:space="preserve">co je </t>
   </si>
   <si>
@@ -1185,6 +1182,9 @@
   </si>
   <si>
     <t>#CO_JE and @PRIBUZNI:táta</t>
+  </si>
+  <si>
+    <t>#CO_JE_MASTER</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1613,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1636,40 +1636,40 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1677,1540 +1677,1540 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>237</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>240</v>
-      </c>
       <c r="E36" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B107" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B112" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="B118" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B135" s="6" t="s">
         <v>317</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B152" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B157" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="B157" s="6" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B158" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B168" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B189" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B199" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="B199" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B209" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="B209" s="6" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B219" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="B219" s="6" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B220" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="B220" s="6" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B221" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="B221" s="6" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B222" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="B222" s="6" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B230" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="B230" s="6" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B231" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="B231" s="6" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B232" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="B232" s="6" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B233" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="B233" s="6" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B270" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="B270" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B271" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="B271" s="6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B272" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="B272" s="6" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B291" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="B291" s="6" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B306" s="6" t="s">
         <v>278</v>
-      </c>
-      <c r="B306" s="6" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B310" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="B310" s="6" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B311" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B312" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B313" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B314" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B315" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A348"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -3234,82 +3234,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -3317,52 +3317,52 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -4104,8 +4104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4146,91 +4146,91 @@
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3"/>

</xml_diff>